<commit_message>
[PHOENIX-5854] - data change to fix trade license automation and added some scenarios
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/grievancesTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/grievancesTestData.xlsx
@@ -68,22 +68,22 @@
     <t>processingStatus</t>
   </si>
   <si>
-    <t>Public Health and Sanitation</t>
-  </si>
-  <si>
-    <t>Dog menace</t>
-  </si>
-  <si>
     <t>Near Vinayaka Temple</t>
   </si>
   <si>
     <t>PROCESSING</t>
   </si>
   <si>
-    <t>Stray dogs are biting. Please catch them</t>
-  </si>
-  <si>
     <t>Avanthi Nagar</t>
+  </si>
+  <si>
+    <t>Non Burning of Street Lights</t>
+  </si>
+  <si>
+    <t>No street light past one week</t>
+  </si>
+  <si>
+    <t>Street Lighting</t>
   </si>
 </sst>
 </file>
@@ -508,7 +508,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +517,7 @@
     <col min="2" max="2" width="27.140625"/>
     <col min="3" max="3" width="27"/>
     <col min="4" max="4" width="24.7109375"/>
-    <col min="5" max="5" width="30.140625"/>
+    <col min="5" max="5" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.5703125"/>
     <col min="7" max="7" width="19.5703125"/>
     <col min="8" max="1025" width="8.5703125"/>
@@ -551,22 +551,22 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>